<commit_message>
chg string operation to buffer.write
</commit_message>
<xml_diff>
--- a/out/09102989061-2.xlsx
+++ b/out/09102989061-2.xlsx
@@ -700,16 +700,17 @@
       <c r="B4" s="6">
         <v>1</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="6" t="s"/>
+      <c r="D4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="7">
+      <c r="F4" s="7">
         <v>110</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>20</v>
       </c>
     </row>
@@ -718,16 +719,17 @@
       <c r="B5" s="6">
         <v>2</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="6" t="s"/>
+      <c r="D5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="7">
+      <c r="F5" s="7">
         <v>-2.7e+01</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -818,16 +820,17 @@
       <c r="B9" s="6">
         <v>1</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="6" t="s"/>
+      <c r="D9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="7">
+      <c r="F9" s="7">
         <v>65</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="G9" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -918,16 +921,17 @@
       <c r="B13" s="6">
         <v>1</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="6" t="s"/>
+      <c r="D13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="7">
+      <c r="F13" s="7">
         <v>20</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="G13" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1018,16 +1022,17 @@
       <c r="B17" s="6">
         <v>1</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="6" t="s"/>
+      <c r="D17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="E17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="7">
+      <c r="F17" s="7">
         <v>130</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="G17" s="6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1118,16 +1123,17 @@
       <c r="B21" s="6">
         <v>1</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="6" t="s"/>
+      <c r="D21" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="E21" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="7">
+      <c r="F21" s="7">
         <v>28</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="G21" s="6" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1218,16 +1224,17 @@
       <c r="B25" s="6">
         <v>1</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="6" t="s"/>
+      <c r="D25" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="E25" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="7">
+      <c r="F25" s="7">
         <v>55</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="G25" s="6" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1318,16 +1325,17 @@
       <c r="B29" s="6">
         <v>1</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="6" t="s"/>
+      <c r="D29" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="E29" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E29" s="7">
+      <c r="F29" s="7">
         <v>70</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="G29" s="6" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1336,16 +1344,17 @@
       <c r="B30" s="6">
         <v>2</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="6" t="s"/>
+      <c r="D30" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="E30" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="7">
+      <c r="F30" s="7">
         <v>-1.1e+01</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="G30" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1354,16 +1363,17 @@
       <c r="B31" s="6">
         <v>3</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="6" t="s"/>
+      <c r="D31" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="E31" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E31" s="7">
+      <c r="F31" s="7">
         <v>30</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="G31" s="6" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1372,16 +1382,17 @@
       <c r="B32" s="6">
         <v>4</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="6" t="s"/>
+      <c r="D32" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="E32" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E32" s="7">
+      <c r="F32" s="7">
         <v>65</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="G32" s="6" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1472,16 +1483,17 @@
       <c r="B36" s="6">
         <v>1</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="6" t="s"/>
+      <c r="D36" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="E36" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E36" s="7">
+      <c r="F36" s="7">
         <v>110</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="G36" s="6" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1490,16 +1502,17 @@
       <c r="B37" s="6">
         <v>2</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="6" t="s"/>
+      <c r="D37" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="E37" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E37" s="7">
+      <c r="F37" s="7">
         <v>-2.7e+01</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="G37" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1508,16 +1521,17 @@
       <c r="B38" s="6">
         <v>3</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="6" t="s"/>
+      <c r="D38" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="E38" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E38" s="7">
+      <c r="F38" s="7">
         <v>-6e+00</v>
       </c>
-      <c r="F38" s="6" t="s">
+      <c r="G38" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1608,16 +1622,17 @@
       <c r="B42" s="6">
         <v>1</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="6" t="s"/>
+      <c r="D42" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="E42" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E42" s="7">
+      <c r="F42" s="7">
         <v>270</v>
       </c>
-      <c r="F42" s="6" t="s">
+      <c r="G42" s="6" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1626,16 +1641,17 @@
       <c r="B43" s="6">
         <v>2</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="6" t="s"/>
+      <c r="D43" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="E43" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E43" s="7">
+      <c r="F43" s="7">
         <v>-3e+01</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="G43" s="6" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1726,16 +1742,17 @@
       <c r="B47" s="6">
         <v>1</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="6" t="s"/>
+      <c r="D47" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="E47" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E47" s="7">
+      <c r="F47" s="7">
         <v>25</v>
       </c>
-      <c r="F47" s="6" t="s">
+      <c r="G47" s="6" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1826,16 +1843,17 @@
       <c r="B51" s="6">
         <v>1</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C51" s="6" t="s"/>
+      <c r="D51" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D51" s="6" t="s">
+      <c r="E51" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E51" s="7">
+      <c r="F51" s="7">
         <v>679</v>
       </c>
-      <c r="F51" s="6" t="s">
+      <c r="G51" s="6" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>